<commit_message>
events dynamically loading into calendar upon click of button correctly.
</commit_message>
<xml_diff>
--- a/OfficeAddIn3/bin/Debug/Book1.xlsx
+++ b/OfficeAddIn3/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R83be6d71af0746e4"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Raf32884971c448c1"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -17,9 +17,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -35,7 +35,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/webextensions/webextension/2010/11">
-              <we:webextensionref xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R4e66172583fe43ff"/>
+              <we:webextensionref xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R2dca5bfb6e104cef"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -47,7 +47,7 @@
             <xdr:cNvPicPr/>
           </xdr:nvPicPr>
           <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="Rada40e3a20e34e51"/>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="Rf1494d2331da4483"/>
             <a:stretch>
               <a:fillRect/>
             </a:stretch>
@@ -66,12 +66,12 @@
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{dee74704-3ef5-455b-9001-8cab27da991a}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{c7e1e6c3-a5f2-4d78-bceb-edce371fecc9}">
   <we:reference id="9061b456-d72a-4138-a6e9-73f25b42e5e4" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>
   <we:bindings/>
-  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="Rada40e3a20e34e51"/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="Rf1494d2331da4483"/>
 </we:webextension>
 </file>
 

</xml_diff>

<commit_message>
replaced date comparison with number comparison, improved performance.
</commit_message>
<xml_diff>
--- a/OfficeAddIn3/bin/Debug/Book1.xlsx
+++ b/OfficeAddIn3/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Raf32884971c448c1"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R7436793b381b43ea"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -35,7 +35,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/webextensions/webextension/2010/11">
-              <we:webextensionref xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R2dca5bfb6e104cef"/>
+              <we:webextensionref xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R9598e07ab30f4953"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -47,7 +47,7 @@
             <xdr:cNvPicPr/>
           </xdr:nvPicPr>
           <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="Rf1494d2331da4483"/>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="Ra1a247d8fbdd476c"/>
             <a:stretch>
               <a:fillRect/>
             </a:stretch>
@@ -66,12 +66,12 @@
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{c7e1e6c3-a5f2-4d78-bceb-edce371fecc9}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{4e298912-5d87-4657-871b-3a7de5d0ed62}">
   <we:reference id="9061b456-d72a-4138-a6e9-73f25b42e5e4" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>
   <we:bindings/>
-  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="Rf1494d2331da4483"/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="Ra1a247d8fbdd476c"/>
 </we:webextension>
 </file>
 

</xml_diff>

<commit_message>
added documentation comments for most functions, the chart now handles null values and supports renaming of the column headers.
</commit_message>
<xml_diff>
--- a/OfficeAddIn3/bin/Debug/Book1.xlsx
+++ b/OfficeAddIn3/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R7436793b381b43ea"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R71f522fda8a24342"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -35,7 +35,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/webextensions/webextension/2010/11">
-              <we:webextensionref xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R9598e07ab30f4953"/>
+              <we:webextensionref xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R0900a4e0deaf4164"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -47,7 +47,7 @@
             <xdr:cNvPicPr/>
           </xdr:nvPicPr>
           <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="Ra1a247d8fbdd476c"/>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="Rd2d46ca99d834d9f"/>
             <a:stretch>
               <a:fillRect/>
             </a:stretch>
@@ -66,12 +66,12 @@
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{4e298912-5d87-4657-871b-3a7de5d0ed62}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{a318240b-960e-4151-8c0f-889a007149da}">
   <we:reference id="9061b456-d72a-4138-a6e9-73f25b42e5e4" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>
   <we:bindings/>
-  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="Ra1a247d8fbdd476c"/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="Rd2d46ca99d834d9f"/>
 </we:webextension>
 </file>
 

</xml_diff>